<commit_message>
feat: added old spike method results in commodity_test_20
</commit_message>
<xml_diff>
--- a/analysis/edcr/Results.xlsx
+++ b/analysis/edcr/Results.xlsx
@@ -432,25 +432,25 @@
         <v>0.001</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C2">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,25 +458,25 @@
         <v>0.002</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C3">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,25 +484,25 @@
         <v>0.003</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C4">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,25 +510,25 @@
         <v>0.004</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C5">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,25 +536,25 @@
         <v>0.005</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C6">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,25 +562,25 @@
         <v>0.006</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C7">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,25 +588,25 @@
         <v>0.007</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C8">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,25 +614,25 @@
         <v>0.008</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C9">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,25 +640,25 @@
         <v>0.009000000000000001</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C10">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,25 +666,25 @@
         <v>0.01</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C11">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,25 +692,25 @@
         <v>0.011</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C12">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,25 +718,25 @@
         <v>0.012</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C13">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,25 +744,25 @@
         <v>0.013</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C14">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,25 +770,25 @@
         <v>0.014</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C15">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,25 +796,25 @@
         <v>0.015</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C16">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,25 +822,25 @@
         <v>0.016</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C17">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,25 +848,25 @@
         <v>0.017</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C18">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,25 +874,25 @@
         <v>0.018</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C19">
-        <v>0.01886792452830189</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0.03703703703703703</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,25 +900,25 @@
         <v>0.019</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G20">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,25 +926,25 @@
         <v>0.02</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,25 +952,25 @@
         <v>0.021</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,25 +978,25 @@
         <v>0.022</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,25 +1004,25 @@
         <v>0.023</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,25 +1030,25 @@
         <v>0.024</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G25">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,25 +1056,25 @@
         <v>0.025</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G26">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,25 +1082,25 @@
         <v>0.026</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G27">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,25 +1108,25 @@
         <v>0.027</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,25 +1134,25 @@
         <v>0.028</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G29">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,25 +1160,25 @@
         <v>0.029</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G30">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,25 +1186,25 @@
         <v>0.03</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,25 +1212,25 @@
         <v>0.031</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,25 +1238,25 @@
         <v>0.032</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,25 +1264,25 @@
         <v>0.033</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G34">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,25 +1290,25 @@
         <v>0.034</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,25 +1316,25 @@
         <v>0.035</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G36">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,25 +1342,25 @@
         <v>0.036</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G37">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,25 +1368,25 @@
         <v>0.037</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,25 +1394,25 @@
         <v>0.038</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G39">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,25 +1420,25 @@
         <v>0.039</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,25 +1446,25 @@
         <v>0.04</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G41">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,25 +1472,25 @@
         <v>0.041</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G42">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,25 +1498,25 @@
         <v>0.042</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G43">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,25 +1524,25 @@
         <v>0.043</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G44">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,25 +1550,25 @@
         <v>0.044</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G45">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,25 +1576,25 @@
         <v>0.045</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G46">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,25 +1602,25 @@
         <v>0.046</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G47">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,25 +1628,25 @@
         <v>0.047</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G48">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,25 +1654,25 @@
         <v>0.048</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,25 +1680,25 @@
         <v>0.049</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,25 +1706,25 @@
         <v>0.05</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G51">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,25 +1732,25 @@
         <v>0.051</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G52">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,25 +1758,25 @@
         <v>0.052</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G53">
         <v>5</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,25 +1784,25 @@
         <v>0.053</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G54">
         <v>5</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,25 +1810,25 @@
         <v>0.054</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G55">
         <v>5</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,25 +1836,25 @@
         <v>0.055</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G56">
         <v>5</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,25 +1862,25 @@
         <v>0.056</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G57">
         <v>5</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,25 +1888,25 @@
         <v>0.057</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G58">
         <v>5</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,25 +1914,25 @@
         <v>0.058</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G59">
         <v>5</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,25 +1940,25 @@
         <v>0.059</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G60">
         <v>5</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,25 +1966,25 @@
         <v>0.06</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G61">
         <v>5</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,25 +1992,25 @@
         <v>0.061</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G62">
         <v>5</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,25 +2018,25 @@
         <v>0.062</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G63">
         <v>5</v>
       </c>
       <c r="H63">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,25 +2044,25 @@
         <v>0.063</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G64">
         <v>5</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,25 +2070,25 @@
         <v>0.064</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G65">
         <v>5</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,25 +2096,25 @@
         <v>0.065</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G66">
         <v>5</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,25 +2122,25 @@
         <v>0.066</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G67">
         <v>5</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,25 +2148,25 @@
         <v>0.067</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G68">
         <v>5</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,25 +2174,25 @@
         <v>0.068</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G69">
         <v>5</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,25 +2200,25 @@
         <v>0.06900000000000001</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G70">
         <v>5</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,25 +2226,25 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G71">
         <v>5</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,25 +2252,25 @@
         <v>0.07100000000000001</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G72">
         <v>5</v>
       </c>
       <c r="H72">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,25 +2278,25 @@
         <v>0.07200000000000001</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G73">
         <v>5</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,25 +2304,25 @@
         <v>0.073</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G74">
         <v>5</v>
       </c>
       <c r="H74">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,25 +2330,25 @@
         <v>0.074</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G75">
         <v>5</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,25 +2356,25 @@
         <v>0.075</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G76">
         <v>5</v>
       </c>
       <c r="H76">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,25 +2382,25 @@
         <v>0.076</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G77">
         <v>5</v>
       </c>
       <c r="H77">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,25 +2408,25 @@
         <v>0.077</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G78">
         <v>5</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,25 +2434,25 @@
         <v>0.078</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G79">
         <v>5</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,25 +2460,25 @@
         <v>0.079</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G80">
         <v>5</v>
       </c>
       <c r="H80">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,25 +2486,25 @@
         <v>0.08</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G81">
         <v>5</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,25 +2512,25 @@
         <v>0.081</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G82">
         <v>5</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,25 +2538,25 @@
         <v>0.082</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G83">
         <v>5</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,25 +2564,25 @@
         <v>0.083</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G84">
         <v>5</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,25 +2590,25 @@
         <v>0.08400000000000001</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G85">
         <v>5</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,25 +2616,25 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E86">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G86">
         <v>5</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,25 +2642,25 @@
         <v>0.08600000000000001</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G87">
         <v>5</v>
       </c>
       <c r="H87">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,25 +2668,25 @@
         <v>0.08700000000000001</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G88">
         <v>5</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,25 +2694,25 @@
         <v>0.08799999999999999</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G89">
         <v>5</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,25 +2720,25 @@
         <v>0.089</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G90">
         <v>5</v>
       </c>
       <c r="H90">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,25 +2746,25 @@
         <v>0.09</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G91">
         <v>5</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,25 +2772,25 @@
         <v>0.091</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G92">
         <v>5</v>
       </c>
       <c r="H92">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,25 +2798,25 @@
         <v>0.092</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G93">
         <v>5</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2824,25 +2824,25 @@
         <v>0.093</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G94">
         <v>5</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2850,25 +2850,25 @@
         <v>0.094</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G95">
         <v>5</v>
       </c>
       <c r="H95">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2876,25 +2876,25 @@
         <v>0.095</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G96">
         <v>5</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2902,25 +2902,25 @@
         <v>0.096</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G97">
         <v>5</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2928,25 +2928,25 @@
         <v>0.097</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E98">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G98">
         <v>5</v>
       </c>
       <c r="H98">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2954,25 +2954,25 @@
         <v>0.098</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G99">
         <v>5</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2980,25 +2980,25 @@
         <v>0.099</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>0.1589041095890411</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>0.2742316784869976</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G100">
         <v>5</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added copper results
</commit_message>
<xml_diff>
--- a/analysis/edcr/Results.xlsx
+++ b/analysis/edcr/Results.xlsx
@@ -432,25 +432,25 @@
         <v>0.001</v>
       </c>
       <c r="B2">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D2">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,25 +458,25 @@
         <v>0.002</v>
       </c>
       <c r="B3">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D3">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,25 +484,25 @@
         <v>0.003</v>
       </c>
       <c r="B4">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D4">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,25 +510,25 @@
         <v>0.004</v>
       </c>
       <c r="B5">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D5">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,25 +536,25 @@
         <v>0.005</v>
       </c>
       <c r="B6">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D6">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,25 +562,25 @@
         <v>0.006</v>
       </c>
       <c r="B7">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D7">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,25 +588,25 @@
         <v>0.007</v>
       </c>
       <c r="B8">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D8">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,25 +614,25 @@
         <v>0.008</v>
       </c>
       <c r="B9">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D9">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,25 +640,25 @@
         <v>0.009000000000000001</v>
       </c>
       <c r="B10">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D10">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,25 +666,25 @@
         <v>0.01</v>
       </c>
       <c r="B11">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D11">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,25 +692,25 @@
         <v>0.011</v>
       </c>
       <c r="B12">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D12">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,25 +718,25 @@
         <v>0.012</v>
       </c>
       <c r="B13">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D13">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,25 +744,25 @@
         <v>0.013</v>
       </c>
       <c r="B14">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D14">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,25 +770,25 @@
         <v>0.014</v>
       </c>
       <c r="B15">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D15">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,25 +796,25 @@
         <v>0.015</v>
       </c>
       <c r="B16">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D16">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,25 +822,25 @@
         <v>0.016</v>
       </c>
       <c r="B17">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D17">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,25 +848,25 @@
         <v>0.017</v>
       </c>
       <c r="B18">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D18">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,25 +874,25 @@
         <v>0.018</v>
       </c>
       <c r="B19">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D19">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,25 +900,25 @@
         <v>0.019</v>
       </c>
       <c r="B20">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D20">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,25 +926,25 @@
         <v>0.02</v>
       </c>
       <c r="B21">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D21">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,25 +952,25 @@
         <v>0.021</v>
       </c>
       <c r="B22">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D22">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,25 +978,25 @@
         <v>0.022</v>
       </c>
       <c r="B23">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D23">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,25 +1004,25 @@
         <v>0.023</v>
       </c>
       <c r="B24">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D24">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,25 +1030,25 @@
         <v>0.024</v>
       </c>
       <c r="B25">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D25">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,25 +1056,25 @@
         <v>0.025</v>
       </c>
       <c r="B26">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D26">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,25 +1082,25 @@
         <v>0.026</v>
       </c>
       <c r="B27">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D27">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,25 +1108,25 @@
         <v>0.027</v>
       </c>
       <c r="B28">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D28">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,25 +1134,25 @@
         <v>0.028</v>
       </c>
       <c r="B29">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D29">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,25 +1160,25 @@
         <v>0.029</v>
       </c>
       <c r="B30">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D30">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,25 +1186,25 @@
         <v>0.03</v>
       </c>
       <c r="B31">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D31">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,25 +1212,25 @@
         <v>0.031</v>
       </c>
       <c r="B32">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D32">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,25 +1238,25 @@
         <v>0.032</v>
       </c>
       <c r="B33">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D33">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,25 +1264,25 @@
         <v>0.033</v>
       </c>
       <c r="B34">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D34">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,25 +1290,25 @@
         <v>0.034</v>
       </c>
       <c r="B35">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D35">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,25 +1316,25 @@
         <v>0.035</v>
       </c>
       <c r="B36">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D36">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,25 +1342,25 @@
         <v>0.036</v>
       </c>
       <c r="B37">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D37">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,25 +1368,25 @@
         <v>0.037</v>
       </c>
       <c r="B38">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D38">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,25 +1394,25 @@
         <v>0.038</v>
       </c>
       <c r="B39">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D39">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,25 +1420,25 @@
         <v>0.039</v>
       </c>
       <c r="B40">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D40">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,25 +1446,25 @@
         <v>0.04</v>
       </c>
       <c r="B41">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D41">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,25 +1472,25 @@
         <v>0.041</v>
       </c>
       <c r="B42">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D42">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,25 +1498,25 @@
         <v>0.042</v>
       </c>
       <c r="B43">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D43">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,25 +1524,25 @@
         <v>0.043</v>
       </c>
       <c r="B44">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D44">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,25 +1550,25 @@
         <v>0.044</v>
       </c>
       <c r="B45">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D45">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,25 +1576,25 @@
         <v>0.045</v>
       </c>
       <c r="B46">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D46">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,25 +1602,25 @@
         <v>0.046</v>
       </c>
       <c r="B47">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D47">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,25 +1628,25 @@
         <v>0.047</v>
       </c>
       <c r="B48">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D48">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,25 +1654,25 @@
         <v>0.048</v>
       </c>
       <c r="B49">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D49">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,25 +1680,25 @@
         <v>0.049</v>
       </c>
       <c r="B50">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D50">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,25 +1706,25 @@
         <v>0.05</v>
       </c>
       <c r="B51">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D51">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,25 +1732,25 @@
         <v>0.051</v>
       </c>
       <c r="B52">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D52">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,25 +1758,25 @@
         <v>0.052</v>
       </c>
       <c r="B53">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D53">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E53">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F53">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G53">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H53">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,25 +1784,25 @@
         <v>0.053</v>
       </c>
       <c r="B54">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D54">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E54">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G54">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H54">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,25 +1810,25 @@
         <v>0.054</v>
       </c>
       <c r="B55">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D55">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E55">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H55">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,25 +1836,25 @@
         <v>0.055</v>
       </c>
       <c r="B56">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D56">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E56">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H56">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,25 +1862,25 @@
         <v>0.056</v>
       </c>
       <c r="B57">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D57">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E57">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F57">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H57">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,25 +1888,25 @@
         <v>0.057</v>
       </c>
       <c r="B58">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D58">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E58">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H58">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,25 +1914,25 @@
         <v>0.058</v>
       </c>
       <c r="B59">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D59">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E59">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G59">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H59">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,25 +1940,25 @@
         <v>0.059</v>
       </c>
       <c r="B60">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D60">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E60">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H60">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,25 +1966,25 @@
         <v>0.06</v>
       </c>
       <c r="B61">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D61">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E61">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G61">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H61">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,25 +1992,25 @@
         <v>0.061</v>
       </c>
       <c r="B62">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D62">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E62">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G62">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H62">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,25 +2018,25 @@
         <v>0.062</v>
       </c>
       <c r="B63">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D63">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E63">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F63">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G63">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H63">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,25 +2044,25 @@
         <v>0.063</v>
       </c>
       <c r="B64">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D64">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E64">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F64">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G64">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H64">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,25 +2070,25 @@
         <v>0.064</v>
       </c>
       <c r="B65">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D65">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E65">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H65">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,25 +2096,25 @@
         <v>0.065</v>
       </c>
       <c r="B66">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D66">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E66">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G66">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H66">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,25 +2122,25 @@
         <v>0.066</v>
       </c>
       <c r="B67">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D67">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E67">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,25 +2148,25 @@
         <v>0.067</v>
       </c>
       <c r="B68">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D68">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E68">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F68">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G68">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H68">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,25 +2174,25 @@
         <v>0.068</v>
       </c>
       <c r="B69">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D69">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E69">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F69">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G69">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H69">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,25 +2200,25 @@
         <v>0.06900000000000001</v>
       </c>
       <c r="B70">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D70">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E70">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F70">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G70">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H70">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,25 +2226,25 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="B71">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D71">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E71">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H71">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,25 +2252,25 @@
         <v>0.07100000000000001</v>
       </c>
       <c r="B72">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D72">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E72">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H72">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,25 +2278,25 @@
         <v>0.07200000000000001</v>
       </c>
       <c r="B73">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D73">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E73">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F73">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G73">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H73">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,25 +2304,25 @@
         <v>0.073</v>
       </c>
       <c r="B74">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D74">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E74">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G74">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H74">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,25 +2330,25 @@
         <v>0.074</v>
       </c>
       <c r="B75">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D75">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E75">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F75">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H75">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,25 +2356,25 @@
         <v>0.075</v>
       </c>
       <c r="B76">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D76">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E76">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F76">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G76">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H76">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,25 +2382,25 @@
         <v>0.076</v>
       </c>
       <c r="B77">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D77">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E77">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F77">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G77">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H77">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,25 +2408,25 @@
         <v>0.077</v>
       </c>
       <c r="B78">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D78">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E78">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G78">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H78">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,25 +2434,25 @@
         <v>0.078</v>
       </c>
       <c r="B79">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D79">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E79">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F79">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G79">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H79">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,25 +2460,25 @@
         <v>0.079</v>
       </c>
       <c r="B80">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D80">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E80">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G80">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H80">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,25 +2486,25 @@
         <v>0.08</v>
       </c>
       <c r="B81">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D81">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E81">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G81">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H81">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,25 +2512,25 @@
         <v>0.081</v>
       </c>
       <c r="B82">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D82">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E82">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F82">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G82">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H82">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,25 +2538,25 @@
         <v>0.082</v>
       </c>
       <c r="B83">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D83">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E83">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G83">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H83">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,25 +2564,25 @@
         <v>0.083</v>
       </c>
       <c r="B84">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D84">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E84">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G84">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H84">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,25 +2590,25 @@
         <v>0.08400000000000001</v>
       </c>
       <c r="B85">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D85">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E85">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G85">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H85">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,25 +2616,25 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="B86">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D86">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E86">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F86">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G86">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H86">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,25 +2642,25 @@
         <v>0.08600000000000001</v>
       </c>
       <c r="B87">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D87">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E87">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G87">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H87">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,25 +2668,25 @@
         <v>0.08700000000000001</v>
       </c>
       <c r="B88">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D88">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E88">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G88">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H88">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,25 +2694,25 @@
         <v>0.08799999999999999</v>
       </c>
       <c r="B89">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D89">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E89">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G89">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H89">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,25 +2720,25 @@
         <v>0.089</v>
       </c>
       <c r="B90">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D90">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E90">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H90">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,25 +2746,25 @@
         <v>0.09</v>
       </c>
       <c r="B91">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D91">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E91">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G91">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H91">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,25 +2772,25 @@
         <v>0.091</v>
       </c>
       <c r="B92">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D92">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E92">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G92">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H92">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,25 +2798,25 @@
         <v>0.092</v>
       </c>
       <c r="B93">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D93">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E93">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G93">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H93">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2824,25 +2824,25 @@
         <v>0.093</v>
       </c>
       <c r="B94">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D94">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E94">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G94">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H94">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2850,25 +2850,25 @@
         <v>0.094</v>
       </c>
       <c r="B95">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D95">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E95">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F95">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G95">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H95">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2876,25 +2876,25 @@
         <v>0.095</v>
       </c>
       <c r="B96">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D96">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E96">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F96">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G96">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H96">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2902,25 +2902,25 @@
         <v>0.096</v>
       </c>
       <c r="B97">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D97">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E97">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F97">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G97">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H97">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2928,25 +2928,25 @@
         <v>0.097</v>
       </c>
       <c r="B98">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D98">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E98">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G98">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H98">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2954,25 +2954,25 @@
         <v>0.098</v>
       </c>
       <c r="B99">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D99">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E99">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G99">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H99">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2980,25 +2980,25 @@
         <v>0.099</v>
       </c>
       <c r="B100">
-        <v>0.1589041095890411</v>
+        <v>0.1808118081180812</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="D100">
-        <v>0.2742316784869976</v>
+        <v>0.2865497076023392</v>
       </c>
       <c r="E100">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="G100">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H100">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added nickel results
</commit_message>
<xml_diff>
--- a/analysis/edcr/Results.xlsx
+++ b/analysis/edcr/Results.xlsx
@@ -432,25 +432,25 @@
         <v>0.001</v>
       </c>
       <c r="B2">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C2">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D2">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,25 +458,25 @@
         <v>0.002</v>
       </c>
       <c r="B3">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C3">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D3">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,25 +484,25 @@
         <v>0.003</v>
       </c>
       <c r="B4">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C4">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D4">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,25 +510,25 @@
         <v>0.004</v>
       </c>
       <c r="B5">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C5">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D5">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,25 +536,25 @@
         <v>0.005</v>
       </c>
       <c r="B6">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C6">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D6">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,25 +562,25 @@
         <v>0.006</v>
       </c>
       <c r="B7">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C7">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D7">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,25 +588,25 @@
         <v>0.007</v>
       </c>
       <c r="B8">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C8">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D8">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,25 +614,25 @@
         <v>0.008</v>
       </c>
       <c r="B9">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C9">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D9">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,25 +640,25 @@
         <v>0.009000000000000001</v>
       </c>
       <c r="B10">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C10">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D10">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,25 +666,25 @@
         <v>0.01</v>
       </c>
       <c r="B11">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C11">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D11">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,25 +692,25 @@
         <v>0.011</v>
       </c>
       <c r="B12">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C12">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D12">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,25 +718,25 @@
         <v>0.012</v>
       </c>
       <c r="B13">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C13">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D13">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,25 +744,25 @@
         <v>0.013</v>
       </c>
       <c r="B14">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C14">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D14">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,25 +770,25 @@
         <v>0.014</v>
       </c>
       <c r="B15">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C15">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D15">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,25 +796,25 @@
         <v>0.015</v>
       </c>
       <c r="B16">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C16">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D16">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,25 +822,25 @@
         <v>0.016</v>
       </c>
       <c r="B17">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C17">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D17">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,25 +848,25 @@
         <v>0.017</v>
       </c>
       <c r="B18">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C18">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D18">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,25 +874,25 @@
         <v>0.018</v>
       </c>
       <c r="B19">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C19">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D19">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,25 +900,25 @@
         <v>0.019</v>
       </c>
       <c r="B20">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C20">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D20">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,25 +926,25 @@
         <v>0.02</v>
       </c>
       <c r="B21">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C21">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D21">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,25 +952,25 @@
         <v>0.021</v>
       </c>
       <c r="B22">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C22">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D22">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,25 +978,25 @@
         <v>0.022</v>
       </c>
       <c r="B23">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C23">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D23">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,25 +1004,25 @@
         <v>0.023</v>
       </c>
       <c r="B24">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C24">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D24">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,25 +1030,25 @@
         <v>0.024</v>
       </c>
       <c r="B25">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C25">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D25">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,25 +1056,25 @@
         <v>0.025</v>
       </c>
       <c r="B26">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C26">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D26">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,25 +1082,25 @@
         <v>0.026</v>
       </c>
       <c r="B27">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C27">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D27">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,25 +1108,25 @@
         <v>0.027</v>
       </c>
       <c r="B28">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C28">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D28">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,25 +1134,25 @@
         <v>0.028</v>
       </c>
       <c r="B29">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C29">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D29">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,25 +1160,25 @@
         <v>0.029</v>
       </c>
       <c r="B30">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C30">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D30">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,25 +1186,25 @@
         <v>0.03</v>
       </c>
       <c r="B31">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C31">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D31">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,25 +1212,25 @@
         <v>0.031</v>
       </c>
       <c r="B32">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C32">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D32">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,25 +1238,25 @@
         <v>0.032</v>
       </c>
       <c r="B33">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C33">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D33">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,25 +1264,25 @@
         <v>0.033</v>
       </c>
       <c r="B34">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C34">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D34">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,25 +1290,25 @@
         <v>0.034</v>
       </c>
       <c r="B35">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C35">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D35">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,25 +1316,25 @@
         <v>0.035</v>
       </c>
       <c r="B36">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C36">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D36">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,25 +1342,25 @@
         <v>0.036</v>
       </c>
       <c r="B37">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C37">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D37">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,25 +1368,25 @@
         <v>0.037</v>
       </c>
       <c r="B38">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C38">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D38">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,25 +1394,25 @@
         <v>0.038</v>
       </c>
       <c r="B39">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C39">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D39">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,25 +1420,25 @@
         <v>0.039</v>
       </c>
       <c r="B40">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C40">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D40">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,25 +1446,25 @@
         <v>0.04</v>
       </c>
       <c r="B41">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C41">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D41">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,25 +1472,25 @@
         <v>0.041</v>
       </c>
       <c r="B42">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C42">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D42">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,25 +1498,25 @@
         <v>0.042</v>
       </c>
       <c r="B43">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C43">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D43">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,25 +1524,25 @@
         <v>0.043</v>
       </c>
       <c r="B44">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C44">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D44">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,25 +1550,25 @@
         <v>0.044</v>
       </c>
       <c r="B45">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C45">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D45">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,25 +1576,25 @@
         <v>0.045</v>
       </c>
       <c r="B46">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C46">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D46">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,25 +1602,25 @@
         <v>0.046</v>
       </c>
       <c r="B47">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C47">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D47">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,25 +1628,25 @@
         <v>0.047</v>
       </c>
       <c r="B48">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C48">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D48">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,25 +1654,25 @@
         <v>0.048</v>
       </c>
       <c r="B49">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C49">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D49">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,25 +1680,25 @@
         <v>0.049</v>
       </c>
       <c r="B50">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C50">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D50">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,25 +1706,25 @@
         <v>0.05</v>
       </c>
       <c r="B51">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C51">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D51">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,25 +1732,25 @@
         <v>0.051</v>
       </c>
       <c r="B52">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C52">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D52">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,25 +1758,25 @@
         <v>0.052</v>
       </c>
       <c r="B53">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C53">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D53">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,25 +1784,25 @@
         <v>0.053</v>
       </c>
       <c r="B54">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C54">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D54">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,25 +1810,25 @@
         <v>0.054</v>
       </c>
       <c r="B55">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C55">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D55">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,25 +1836,25 @@
         <v>0.055</v>
       </c>
       <c r="B56">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C56">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D56">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,25 +1862,25 @@
         <v>0.056</v>
       </c>
       <c r="B57">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C57">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D57">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,25 +1888,25 @@
         <v>0.057</v>
       </c>
       <c r="B58">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C58">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D58">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,25 +1914,25 @@
         <v>0.058</v>
       </c>
       <c r="B59">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C59">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D59">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,25 +1940,25 @@
         <v>0.059</v>
       </c>
       <c r="B60">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C60">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D60">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,25 +1966,25 @@
         <v>0.06</v>
       </c>
       <c r="B61">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C61">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D61">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,25 +1992,25 @@
         <v>0.061</v>
       </c>
       <c r="B62">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C62">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D62">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,25 +2018,25 @@
         <v>0.062</v>
       </c>
       <c r="B63">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C63">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D63">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,25 +2044,25 @@
         <v>0.063</v>
       </c>
       <c r="B64">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C64">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D64">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,25 +2070,25 @@
         <v>0.064</v>
       </c>
       <c r="B65">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C65">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D65">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,25 +2096,25 @@
         <v>0.065</v>
       </c>
       <c r="B66">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C66">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D66">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,25 +2122,25 @@
         <v>0.066</v>
       </c>
       <c r="B67">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C67">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D67">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G67">
         <v>0</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,25 +2148,25 @@
         <v>0.067</v>
       </c>
       <c r="B68">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C68">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D68">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,25 +2174,25 @@
         <v>0.068</v>
       </c>
       <c r="B69">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C69">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D69">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G69">
         <v>0</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,25 +2200,25 @@
         <v>0.06900000000000001</v>
       </c>
       <c r="B70">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C70">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D70">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G70">
         <v>0</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,25 +2226,25 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="B71">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C71">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D71">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G71">
         <v>0</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,25 +2252,25 @@
         <v>0.07100000000000001</v>
       </c>
       <c r="B72">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C72">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D72">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G72">
         <v>0</v>
       </c>
       <c r="H72">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,25 +2278,25 @@
         <v>0.07200000000000001</v>
       </c>
       <c r="B73">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C73">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D73">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G73">
         <v>0</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,25 +2304,25 @@
         <v>0.073</v>
       </c>
       <c r="B74">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C74">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D74">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G74">
         <v>0</v>
       </c>
       <c r="H74">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,25 +2330,25 @@
         <v>0.074</v>
       </c>
       <c r="B75">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C75">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D75">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G75">
         <v>0</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,25 +2356,25 @@
         <v>0.075</v>
       </c>
       <c r="B76">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C76">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D76">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G76">
         <v>0</v>
       </c>
       <c r="H76">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,25 +2382,25 @@
         <v>0.076</v>
       </c>
       <c r="B77">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C77">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D77">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G77">
         <v>0</v>
       </c>
       <c r="H77">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,25 +2408,25 @@
         <v>0.077</v>
       </c>
       <c r="B78">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C78">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D78">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G78">
         <v>0</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,25 +2434,25 @@
         <v>0.078</v>
       </c>
       <c r="B79">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C79">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D79">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E79">
         <v>0</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G79">
         <v>0</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,25 +2460,25 @@
         <v>0.079</v>
       </c>
       <c r="B80">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C80">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D80">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E80">
         <v>0</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G80">
         <v>0</v>
       </c>
       <c r="H80">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,25 +2486,25 @@
         <v>0.08</v>
       </c>
       <c r="B81">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C81">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D81">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G81">
         <v>0</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,25 +2512,25 @@
         <v>0.081</v>
       </c>
       <c r="B82">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C82">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D82">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G82">
         <v>0</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,25 +2538,25 @@
         <v>0.082</v>
       </c>
       <c r="B83">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C83">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D83">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E83">
         <v>0</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G83">
         <v>0</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,25 +2564,25 @@
         <v>0.083</v>
       </c>
       <c r="B84">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C84">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D84">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G84">
         <v>0</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,25 +2590,25 @@
         <v>0.08400000000000001</v>
       </c>
       <c r="B85">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C85">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D85">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G85">
         <v>0</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,25 +2616,25 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="B86">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C86">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D86">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G86">
         <v>0</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,25 +2642,25 @@
         <v>0.08600000000000001</v>
       </c>
       <c r="B87">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C87">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D87">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E87">
         <v>0</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G87">
         <v>0</v>
       </c>
       <c r="H87">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,25 +2668,25 @@
         <v>0.08700000000000001</v>
       </c>
       <c r="B88">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C88">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D88">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G88">
         <v>0</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,25 +2694,25 @@
         <v>0.08799999999999999</v>
       </c>
       <c r="B89">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C89">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D89">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G89">
         <v>0</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,25 +2720,25 @@
         <v>0.089</v>
       </c>
       <c r="B90">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C90">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D90">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G90">
         <v>0</v>
       </c>
       <c r="H90">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,25 +2746,25 @@
         <v>0.09</v>
       </c>
       <c r="B91">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C91">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D91">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G91">
         <v>0</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,25 +2772,25 @@
         <v>0.091</v>
       </c>
       <c r="B92">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C92">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D92">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G92">
         <v>0</v>
       </c>
       <c r="H92">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,25 +2798,25 @@
         <v>0.092</v>
       </c>
       <c r="B93">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C93">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D93">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E93">
         <v>0</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G93">
         <v>0</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2824,25 +2824,25 @@
         <v>0.093</v>
       </c>
       <c r="B94">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C94">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D94">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E94">
         <v>0</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G94">
         <v>0</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2850,25 +2850,25 @@
         <v>0.094</v>
       </c>
       <c r="B95">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C95">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D95">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G95">
         <v>0</v>
       </c>
       <c r="H95">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2876,25 +2876,25 @@
         <v>0.095</v>
       </c>
       <c r="B96">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C96">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D96">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G96">
         <v>0</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2902,25 +2902,25 @@
         <v>0.096</v>
       </c>
       <c r="B97">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C97">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D97">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G97">
         <v>0</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2928,25 +2928,25 @@
         <v>0.097</v>
       </c>
       <c r="B98">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C98">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D98">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E98">
         <v>0</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G98">
         <v>0</v>
       </c>
       <c r="H98">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2954,25 +2954,25 @@
         <v>0.098</v>
       </c>
       <c r="B99">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C99">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D99">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G99">
         <v>0</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2980,25 +2980,25 @@
         <v>0.099</v>
       </c>
       <c r="B100">
-        <v>0.1808118081180812</v>
+        <v>0.18125</v>
       </c>
       <c r="C100">
-        <v>0.6901408450704225</v>
+        <v>0.4603174603174603</v>
       </c>
       <c r="D100">
-        <v>0.2865497076023392</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G100">
         <v>0</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added threshold and model exclusion function
</commit_message>
<xml_diff>
--- a/analysis/edcr/Results.xlsx
+++ b/analysis/edcr/Results.xlsx
@@ -432,25 +432,25 @@
         <v>0.001</v>
       </c>
       <c r="B2">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C2">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D2">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,25 +458,25 @@
         <v>0.002</v>
       </c>
       <c r="B3">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C3">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D3">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,25 +484,25 @@
         <v>0.003</v>
       </c>
       <c r="B4">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C4">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D4">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,25 +510,25 @@
         <v>0.004</v>
       </c>
       <c r="B5">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C5">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D5">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,25 +536,25 @@
         <v>0.005</v>
       </c>
       <c r="B6">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C6">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D6">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,25 +562,25 @@
         <v>0.006</v>
       </c>
       <c r="B7">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C7">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D7">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,25 +588,25 @@
         <v>0.007</v>
       </c>
       <c r="B8">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C8">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D8">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,25 +614,25 @@
         <v>0.008</v>
       </c>
       <c r="B9">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C9">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D9">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,25 +640,25 @@
         <v>0.009000000000000001</v>
       </c>
       <c r="B10">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C10">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D10">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,25 +666,25 @@
         <v>0.01</v>
       </c>
       <c r="B11">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C11">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D11">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,25 +692,25 @@
         <v>0.011</v>
       </c>
       <c r="B12">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C12">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D12">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,25 +718,25 @@
         <v>0.012</v>
       </c>
       <c r="B13">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C13">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D13">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,25 +744,25 @@
         <v>0.013</v>
       </c>
       <c r="B14">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C14">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D14">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,25 +770,25 @@
         <v>0.014</v>
       </c>
       <c r="B15">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C15">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D15">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,25 +796,25 @@
         <v>0.015</v>
       </c>
       <c r="B16">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C16">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D16">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,25 +822,25 @@
         <v>0.016</v>
       </c>
       <c r="B17">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C17">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D17">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,25 +848,25 @@
         <v>0.017</v>
       </c>
       <c r="B18">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C18">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D18">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,25 +874,25 @@
         <v>0.018</v>
       </c>
       <c r="B19">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C19">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D19">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,25 +900,25 @@
         <v>0.019</v>
       </c>
       <c r="B20">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C20">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D20">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,25 +926,25 @@
         <v>0.02</v>
       </c>
       <c r="B21">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C21">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D21">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,25 +952,25 @@
         <v>0.021</v>
       </c>
       <c r="B22">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C22">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D22">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,25 +978,25 @@
         <v>0.022</v>
       </c>
       <c r="B23">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C23">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D23">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,25 +1004,25 @@
         <v>0.023</v>
       </c>
       <c r="B24">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C24">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D24">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,25 +1030,25 @@
         <v>0.024</v>
       </c>
       <c r="B25">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C25">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D25">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,25 +1056,25 @@
         <v>0.025</v>
       </c>
       <c r="B26">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C26">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D26">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,25 +1082,25 @@
         <v>0.026</v>
       </c>
       <c r="B27">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C27">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D27">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,25 +1108,25 @@
         <v>0.027</v>
       </c>
       <c r="B28">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C28">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D28">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,25 +1134,25 @@
         <v>0.028</v>
       </c>
       <c r="B29">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C29">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D29">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,25 +1160,25 @@
         <v>0.029</v>
       </c>
       <c r="B30">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C30">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D30">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,25 +1186,25 @@
         <v>0.03</v>
       </c>
       <c r="B31">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C31">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D31">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,25 +1212,25 @@
         <v>0.031</v>
       </c>
       <c r="B32">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C32">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D32">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,25 +1238,25 @@
         <v>0.032</v>
       </c>
       <c r="B33">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C33">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D33">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,25 +1264,25 @@
         <v>0.033</v>
       </c>
       <c r="B34">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C34">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D34">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,25 +1290,25 @@
         <v>0.034</v>
       </c>
       <c r="B35">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C35">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D35">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,25 +1316,25 @@
         <v>0.035</v>
       </c>
       <c r="B36">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C36">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D36">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,25 +1342,25 @@
         <v>0.036</v>
       </c>
       <c r="B37">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C37">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D37">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,25 +1368,25 @@
         <v>0.037</v>
       </c>
       <c r="B38">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C38">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D38">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,25 +1394,25 @@
         <v>0.038</v>
       </c>
       <c r="B39">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C39">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D39">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,25 +1420,25 @@
         <v>0.039</v>
       </c>
       <c r="B40">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C40">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D40">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,25 +1446,25 @@
         <v>0.04</v>
       </c>
       <c r="B41">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C41">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D41">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,25 +1472,25 @@
         <v>0.041</v>
       </c>
       <c r="B42">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C42">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D42">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,25 +1498,25 @@
         <v>0.042</v>
       </c>
       <c r="B43">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C43">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D43">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,25 +1524,25 @@
         <v>0.043</v>
       </c>
       <c r="B44">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C44">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D44">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,25 +1550,25 @@
         <v>0.044</v>
       </c>
       <c r="B45">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C45">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D45">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,25 +1576,25 @@
         <v>0.045</v>
       </c>
       <c r="B46">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C46">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D46">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,25 +1602,25 @@
         <v>0.046</v>
       </c>
       <c r="B47">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C47">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D47">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,25 +1628,25 @@
         <v>0.047</v>
       </c>
       <c r="B48">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C48">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D48">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,25 +1654,25 @@
         <v>0.048</v>
       </c>
       <c r="B49">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C49">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D49">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,25 +1680,25 @@
         <v>0.049</v>
       </c>
       <c r="B50">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C50">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D50">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,25 +1706,25 @@
         <v>0.05</v>
       </c>
       <c r="B51">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C51">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D51">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,25 +1732,25 @@
         <v>0.051</v>
       </c>
       <c r="B52">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C52">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D52">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,25 +1758,25 @@
         <v>0.052</v>
       </c>
       <c r="B53">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C53">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D53">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,25 +1784,25 @@
         <v>0.053</v>
       </c>
       <c r="B54">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C54">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D54">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,25 +1810,25 @@
         <v>0.054</v>
       </c>
       <c r="B55">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C55">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D55">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,25 +1836,25 @@
         <v>0.055</v>
       </c>
       <c r="B56">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C56">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D56">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,25 +1862,25 @@
         <v>0.056</v>
       </c>
       <c r="B57">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C57">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D57">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,25 +1888,25 @@
         <v>0.057</v>
       </c>
       <c r="B58">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C58">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D58">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,25 +1914,25 @@
         <v>0.058</v>
       </c>
       <c r="B59">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C59">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D59">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,25 +1940,25 @@
         <v>0.059</v>
       </c>
       <c r="B60">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C60">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D60">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,25 +1966,25 @@
         <v>0.06</v>
       </c>
       <c r="B61">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C61">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D61">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,25 +1992,25 @@
         <v>0.061</v>
       </c>
       <c r="B62">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C62">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D62">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,25 +2018,25 @@
         <v>0.062</v>
       </c>
       <c r="B63">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C63">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D63">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,25 +2044,25 @@
         <v>0.063</v>
       </c>
       <c r="B64">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C64">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D64">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,25 +2070,25 @@
         <v>0.064</v>
       </c>
       <c r="B65">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C65">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D65">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,25 +2096,25 @@
         <v>0.065</v>
       </c>
       <c r="B66">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C66">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D66">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,25 +2122,25 @@
         <v>0.066</v>
       </c>
       <c r="B67">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C67">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D67">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F67">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H67">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,25 +2148,25 @@
         <v>0.067</v>
       </c>
       <c r="B68">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C68">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D68">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F68">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H68">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,25 +2174,25 @@
         <v>0.068</v>
       </c>
       <c r="B69">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C69">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D69">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F69">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H69">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,25 +2200,25 @@
         <v>0.06900000000000001</v>
       </c>
       <c r="B70">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C70">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D70">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F70">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H70">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,25 +2226,25 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="B71">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C71">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D71">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F71">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H71">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,25 +2252,25 @@
         <v>0.07100000000000001</v>
       </c>
       <c r="B72">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C72">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D72">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F72">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H72">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,25 +2278,25 @@
         <v>0.07200000000000001</v>
       </c>
       <c r="B73">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C73">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D73">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F73">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H73">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,25 +2304,25 @@
         <v>0.073</v>
       </c>
       <c r="B74">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C74">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D74">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F74">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H74">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,25 +2330,25 @@
         <v>0.074</v>
       </c>
       <c r="B75">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C75">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D75">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F75">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H75">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,25 +2356,25 @@
         <v>0.075</v>
       </c>
       <c r="B76">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C76">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D76">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F76">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H76">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,25 +2382,25 @@
         <v>0.076</v>
       </c>
       <c r="B77">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C77">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D77">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F77">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H77">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,25 +2408,25 @@
         <v>0.077</v>
       </c>
       <c r="B78">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C78">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D78">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F78">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H78">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,25 +2434,25 @@
         <v>0.078</v>
       </c>
       <c r="B79">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C79">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D79">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F79">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H79">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,25 +2460,25 @@
         <v>0.079</v>
       </c>
       <c r="B80">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C80">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D80">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F80">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H80">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,25 +2486,25 @@
         <v>0.08</v>
       </c>
       <c r="B81">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C81">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D81">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F81">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H81">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,25 +2512,25 @@
         <v>0.081</v>
       </c>
       <c r="B82">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C82">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D82">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F82">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H82">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,25 +2538,25 @@
         <v>0.082</v>
       </c>
       <c r="B83">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C83">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D83">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F83">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H83">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,25 +2564,25 @@
         <v>0.083</v>
       </c>
       <c r="B84">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C84">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D84">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F84">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H84">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,25 +2590,25 @@
         <v>0.08400000000000001</v>
       </c>
       <c r="B85">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C85">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D85">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F85">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H85">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,25 +2616,25 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="B86">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C86">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D86">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F86">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H86">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,25 +2642,25 @@
         <v>0.08600000000000001</v>
       </c>
       <c r="B87">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C87">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D87">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F87">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H87">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,25 +2668,25 @@
         <v>0.08700000000000001</v>
       </c>
       <c r="B88">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C88">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D88">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F88">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H88">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,25 +2694,25 @@
         <v>0.08799999999999999</v>
       </c>
       <c r="B89">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C89">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D89">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F89">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H89">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,25 +2720,25 @@
         <v>0.089</v>
       </c>
       <c r="B90">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C90">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D90">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F90">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H90">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,25 +2746,25 @@
         <v>0.09</v>
       </c>
       <c r="B91">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C91">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D91">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F91">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H91">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,25 +2772,25 @@
         <v>0.091</v>
       </c>
       <c r="B92">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C92">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D92">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F92">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H92">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,25 +2798,25 @@
         <v>0.092</v>
       </c>
       <c r="B93">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C93">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D93">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F93">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H93">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2824,25 +2824,25 @@
         <v>0.093</v>
       </c>
       <c r="B94">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C94">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D94">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F94">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H94">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2850,25 +2850,25 @@
         <v>0.094</v>
       </c>
       <c r="B95">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C95">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D95">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F95">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H95">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2876,25 +2876,25 @@
         <v>0.095</v>
       </c>
       <c r="B96">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C96">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D96">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E96">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F96">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H96">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2902,25 +2902,25 @@
         <v>0.096</v>
       </c>
       <c r="B97">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C97">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D97">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F97">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H97">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2928,25 +2928,25 @@
         <v>0.097</v>
       </c>
       <c r="B98">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C98">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D98">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F98">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H98">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2954,25 +2954,25 @@
         <v>0.098</v>
       </c>
       <c r="B99">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C99">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D99">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F99">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H99">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2980,25 +2980,25 @@
         <v>0.099</v>
       </c>
       <c r="B100">
-        <v>0.18125</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C100">
-        <v>0.4603174603174603</v>
+        <v>0.4262295081967213</v>
       </c>
       <c r="D100">
-        <v>0.2600896860986547</v>
+        <v>0.3058823529411765</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F100">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G100">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H100">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: slightly adjusted the filtering function
</commit_message>
<xml_diff>
--- a/analysis/edcr/Results.xlsx
+++ b/analysis/edcr/Results.xlsx
@@ -432,25 +432,25 @@
         <v>0.001</v>
       </c>
       <c r="B2">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C2">
         <v>0.4262295081967213</v>
       </c>
       <c r="D2">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,25 +458,25 @@
         <v>0.002</v>
       </c>
       <c r="B3">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C3">
         <v>0.4262295081967213</v>
       </c>
       <c r="D3">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,25 +484,25 @@
         <v>0.003</v>
       </c>
       <c r="B4">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C4">
         <v>0.4262295081967213</v>
       </c>
       <c r="D4">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,25 +510,25 @@
         <v>0.004</v>
       </c>
       <c r="B5">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C5">
         <v>0.4262295081967213</v>
       </c>
       <c r="D5">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,25 +536,25 @@
         <v>0.005</v>
       </c>
       <c r="B6">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C6">
         <v>0.4262295081967213</v>
       </c>
       <c r="D6">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,25 +562,25 @@
         <v>0.006</v>
       </c>
       <c r="B7">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C7">
         <v>0.4262295081967213</v>
       </c>
       <c r="D7">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,25 +588,25 @@
         <v>0.007</v>
       </c>
       <c r="B8">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C8">
         <v>0.4262295081967213</v>
       </c>
       <c r="D8">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,25 +614,25 @@
         <v>0.008</v>
       </c>
       <c r="B9">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C9">
         <v>0.4262295081967213</v>
       </c>
       <c r="D9">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,25 +640,25 @@
         <v>0.009000000000000001</v>
       </c>
       <c r="B10">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C10">
         <v>0.4262295081967213</v>
       </c>
       <c r="D10">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,25 +666,25 @@
         <v>0.01</v>
       </c>
       <c r="B11">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C11">
         <v>0.4262295081967213</v>
       </c>
       <c r="D11">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,25 +692,25 @@
         <v>0.011</v>
       </c>
       <c r="B12">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C12">
         <v>0.4262295081967213</v>
       </c>
       <c r="D12">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,25 +718,25 @@
         <v>0.012</v>
       </c>
       <c r="B13">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C13">
         <v>0.4262295081967213</v>
       </c>
       <c r="D13">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,25 +744,25 @@
         <v>0.013</v>
       </c>
       <c r="B14">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C14">
         <v>0.4262295081967213</v>
       </c>
       <c r="D14">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,25 +770,25 @@
         <v>0.014</v>
       </c>
       <c r="B15">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C15">
         <v>0.4262295081967213</v>
       </c>
       <c r="D15">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,25 +796,25 @@
         <v>0.015</v>
       </c>
       <c r="B16">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C16">
         <v>0.4262295081967213</v>
       </c>
       <c r="D16">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,25 +822,25 @@
         <v>0.016</v>
       </c>
       <c r="B17">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C17">
         <v>0.4262295081967213</v>
       </c>
       <c r="D17">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,25 +848,25 @@
         <v>0.017</v>
       </c>
       <c r="B18">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C18">
         <v>0.4262295081967213</v>
       </c>
       <c r="D18">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,25 +874,25 @@
         <v>0.018</v>
       </c>
       <c r="B19">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C19">
         <v>0.4262295081967213</v>
       </c>
       <c r="D19">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,25 +900,25 @@
         <v>0.019</v>
       </c>
       <c r="B20">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C20">
         <v>0.4262295081967213</v>
       </c>
       <c r="D20">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,25 +926,25 @@
         <v>0.02</v>
       </c>
       <c r="B21">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C21">
         <v>0.4262295081967213</v>
       </c>
       <c r="D21">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,25 +952,25 @@
         <v>0.021</v>
       </c>
       <c r="B22">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C22">
         <v>0.4262295081967213</v>
       </c>
       <c r="D22">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,25 +978,25 @@
         <v>0.022</v>
       </c>
       <c r="B23">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C23">
         <v>0.4262295081967213</v>
       </c>
       <c r="D23">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,25 +1004,25 @@
         <v>0.023</v>
       </c>
       <c r="B24">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C24">
         <v>0.4262295081967213</v>
       </c>
       <c r="D24">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,25 +1030,25 @@
         <v>0.024</v>
       </c>
       <c r="B25">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C25">
         <v>0.4262295081967213</v>
       </c>
       <c r="D25">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,25 +1056,25 @@
         <v>0.025</v>
       </c>
       <c r="B26">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C26">
         <v>0.4262295081967213</v>
       </c>
       <c r="D26">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,25 +1082,25 @@
         <v>0.026</v>
       </c>
       <c r="B27">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C27">
         <v>0.4262295081967213</v>
       </c>
       <c r="D27">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,25 +1108,25 @@
         <v>0.027</v>
       </c>
       <c r="B28">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C28">
         <v>0.4262295081967213</v>
       </c>
       <c r="D28">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,25 +1134,25 @@
         <v>0.028</v>
       </c>
       <c r="B29">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C29">
         <v>0.4262295081967213</v>
       </c>
       <c r="D29">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,25 +1160,25 @@
         <v>0.029</v>
       </c>
       <c r="B30">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C30">
         <v>0.4262295081967213</v>
       </c>
       <c r="D30">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,25 +1186,25 @@
         <v>0.03</v>
       </c>
       <c r="B31">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C31">
         <v>0.4262295081967213</v>
       </c>
       <c r="D31">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,25 +1212,25 @@
         <v>0.031</v>
       </c>
       <c r="B32">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C32">
         <v>0.4262295081967213</v>
       </c>
       <c r="D32">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,25 +1238,25 @@
         <v>0.032</v>
       </c>
       <c r="B33">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C33">
         <v>0.4262295081967213</v>
       </c>
       <c r="D33">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,25 +1264,25 @@
         <v>0.033</v>
       </c>
       <c r="B34">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C34">
         <v>0.4262295081967213</v>
       </c>
       <c r="D34">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,25 +1290,25 @@
         <v>0.034</v>
       </c>
       <c r="B35">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C35">
         <v>0.4262295081967213</v>
       </c>
       <c r="D35">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,25 +1316,25 @@
         <v>0.035</v>
       </c>
       <c r="B36">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C36">
         <v>0.4262295081967213</v>
       </c>
       <c r="D36">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,25 +1342,25 @@
         <v>0.036</v>
       </c>
       <c r="B37">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C37">
         <v>0.4262295081967213</v>
       </c>
       <c r="D37">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,25 +1368,25 @@
         <v>0.037</v>
       </c>
       <c r="B38">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C38">
         <v>0.4262295081967213</v>
       </c>
       <c r="D38">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,25 +1394,25 @@
         <v>0.038</v>
       </c>
       <c r="B39">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C39">
         <v>0.4262295081967213</v>
       </c>
       <c r="D39">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,25 +1420,25 @@
         <v>0.039</v>
       </c>
       <c r="B40">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C40">
         <v>0.4262295081967213</v>
       </c>
       <c r="D40">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,25 +1446,25 @@
         <v>0.04</v>
       </c>
       <c r="B41">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C41">
         <v>0.4262295081967213</v>
       </c>
       <c r="D41">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,25 +1472,25 @@
         <v>0.041</v>
       </c>
       <c r="B42">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C42">
         <v>0.4262295081967213</v>
       </c>
       <c r="D42">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,25 +1498,25 @@
         <v>0.042</v>
       </c>
       <c r="B43">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C43">
         <v>0.4262295081967213</v>
       </c>
       <c r="D43">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,25 +1524,25 @@
         <v>0.043</v>
       </c>
       <c r="B44">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C44">
         <v>0.4262295081967213</v>
       </c>
       <c r="D44">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,25 +1550,25 @@
         <v>0.044</v>
       </c>
       <c r="B45">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C45">
         <v>0.4262295081967213</v>
       </c>
       <c r="D45">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,25 +1576,25 @@
         <v>0.045</v>
       </c>
       <c r="B46">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C46">
         <v>0.4262295081967213</v>
       </c>
       <c r="D46">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,25 +1602,25 @@
         <v>0.046</v>
       </c>
       <c r="B47">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C47">
         <v>0.4262295081967213</v>
       </c>
       <c r="D47">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,25 +1628,25 @@
         <v>0.047</v>
       </c>
       <c r="B48">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C48">
         <v>0.4262295081967213</v>
       </c>
       <c r="D48">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,25 +1654,25 @@
         <v>0.048</v>
       </c>
       <c r="B49">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C49">
         <v>0.4262295081967213</v>
       </c>
       <c r="D49">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,25 +1680,25 @@
         <v>0.049</v>
       </c>
       <c r="B50">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C50">
         <v>0.4262295081967213</v>
       </c>
       <c r="D50">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,25 +1706,25 @@
         <v>0.05</v>
       </c>
       <c r="B51">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C51">
         <v>0.4262295081967213</v>
       </c>
       <c r="D51">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,25 +1732,25 @@
         <v>0.051</v>
       </c>
       <c r="B52">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C52">
         <v>0.4262295081967213</v>
       </c>
       <c r="D52">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,25 +1758,25 @@
         <v>0.052</v>
       </c>
       <c r="B53">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C53">
         <v>0.4262295081967213</v>
       </c>
       <c r="D53">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,25 +1784,25 @@
         <v>0.053</v>
       </c>
       <c r="B54">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C54">
         <v>0.4262295081967213</v>
       </c>
       <c r="D54">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,25 +1810,25 @@
         <v>0.054</v>
       </c>
       <c r="B55">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C55">
         <v>0.4262295081967213</v>
       </c>
       <c r="D55">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,25 +1836,25 @@
         <v>0.055</v>
       </c>
       <c r="B56">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C56">
         <v>0.4262295081967213</v>
       </c>
       <c r="D56">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,25 +1862,25 @@
         <v>0.056</v>
       </c>
       <c r="B57">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C57">
         <v>0.4262295081967213</v>
       </c>
       <c r="D57">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,25 +1888,25 @@
         <v>0.057</v>
       </c>
       <c r="B58">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C58">
         <v>0.4262295081967213</v>
       </c>
       <c r="D58">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,25 +1914,25 @@
         <v>0.058</v>
       </c>
       <c r="B59">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C59">
         <v>0.4262295081967213</v>
       </c>
       <c r="D59">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,25 +1940,25 @@
         <v>0.059</v>
       </c>
       <c r="B60">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C60">
         <v>0.4262295081967213</v>
       </c>
       <c r="D60">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,25 +1966,25 @@
         <v>0.06</v>
       </c>
       <c r="B61">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C61">
         <v>0.4262295081967213</v>
       </c>
       <c r="D61">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,25 +1992,25 @@
         <v>0.061</v>
       </c>
       <c r="B62">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C62">
         <v>0.4262295081967213</v>
       </c>
       <c r="D62">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,25 +2018,25 @@
         <v>0.062</v>
       </c>
       <c r="B63">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C63">
         <v>0.4262295081967213</v>
       </c>
       <c r="D63">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,25 +2044,25 @@
         <v>0.063</v>
       </c>
       <c r="B64">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C64">
         <v>0.4262295081967213</v>
       </c>
       <c r="D64">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,25 +2070,25 @@
         <v>0.064</v>
       </c>
       <c r="B65">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C65">
         <v>0.4262295081967213</v>
       </c>
       <c r="D65">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,25 +2096,25 @@
         <v>0.065</v>
       </c>
       <c r="B66">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C66">
         <v>0.4262295081967213</v>
       </c>
       <c r="D66">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,25 +2122,25 @@
         <v>0.066</v>
       </c>
       <c r="B67">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C67">
         <v>0.4262295081967213</v>
       </c>
       <c r="D67">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E67">
         <v>28</v>
       </c>
       <c r="F67">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G67">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H67">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,25 +2148,25 @@
         <v>0.067</v>
       </c>
       <c r="B68">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C68">
         <v>0.4262295081967213</v>
       </c>
       <c r="D68">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E68">
         <v>28</v>
       </c>
       <c r="F68">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G68">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H68">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,25 +2174,25 @@
         <v>0.068</v>
       </c>
       <c r="B69">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C69">
         <v>0.4262295081967213</v>
       </c>
       <c r="D69">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E69">
         <v>28</v>
       </c>
       <c r="F69">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G69">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H69">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,25 +2200,25 @@
         <v>0.06900000000000001</v>
       </c>
       <c r="B70">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C70">
         <v>0.4262295081967213</v>
       </c>
       <c r="D70">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E70">
         <v>28</v>
       </c>
       <c r="F70">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G70">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H70">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,25 +2226,25 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="B71">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C71">
         <v>0.4262295081967213</v>
       </c>
       <c r="D71">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E71">
         <v>28</v>
       </c>
       <c r="F71">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G71">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H71">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,25 +2252,25 @@
         <v>0.07100000000000001</v>
       </c>
       <c r="B72">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C72">
         <v>0.4262295081967213</v>
       </c>
       <c r="D72">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E72">
         <v>28</v>
       </c>
       <c r="F72">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G72">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H72">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,25 +2278,25 @@
         <v>0.07200000000000001</v>
       </c>
       <c r="B73">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C73">
         <v>0.4262295081967213</v>
       </c>
       <c r="D73">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E73">
         <v>28</v>
       </c>
       <c r="F73">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G73">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H73">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,25 +2304,25 @@
         <v>0.073</v>
       </c>
       <c r="B74">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C74">
         <v>0.4262295081967213</v>
       </c>
       <c r="D74">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E74">
         <v>28</v>
       </c>
       <c r="F74">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G74">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H74">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,25 +2330,25 @@
         <v>0.074</v>
       </c>
       <c r="B75">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C75">
         <v>0.4262295081967213</v>
       </c>
       <c r="D75">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E75">
         <v>28</v>
       </c>
       <c r="F75">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G75">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H75">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,25 +2356,25 @@
         <v>0.075</v>
       </c>
       <c r="B76">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C76">
         <v>0.4262295081967213</v>
       </c>
       <c r="D76">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E76">
         <v>28</v>
       </c>
       <c r="F76">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G76">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H76">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,25 +2382,25 @@
         <v>0.076</v>
       </c>
       <c r="B77">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C77">
         <v>0.4262295081967213</v>
       </c>
       <c r="D77">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E77">
         <v>28</v>
       </c>
       <c r="F77">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G77">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H77">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,25 +2408,25 @@
         <v>0.077</v>
       </c>
       <c r="B78">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C78">
         <v>0.4262295081967213</v>
       </c>
       <c r="D78">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E78">
         <v>28</v>
       </c>
       <c r="F78">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G78">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H78">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,25 +2434,25 @@
         <v>0.078</v>
       </c>
       <c r="B79">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C79">
         <v>0.4262295081967213</v>
       </c>
       <c r="D79">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E79">
         <v>28</v>
       </c>
       <c r="F79">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G79">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H79">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,25 +2460,25 @@
         <v>0.079</v>
       </c>
       <c r="B80">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C80">
         <v>0.4262295081967213</v>
       </c>
       <c r="D80">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E80">
         <v>28</v>
       </c>
       <c r="F80">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G80">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H80">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,25 +2486,25 @@
         <v>0.08</v>
       </c>
       <c r="B81">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C81">
         <v>0.4262295081967213</v>
       </c>
       <c r="D81">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E81">
         <v>28</v>
       </c>
       <c r="F81">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G81">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H81">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,25 +2512,25 @@
         <v>0.081</v>
       </c>
       <c r="B82">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C82">
         <v>0.4262295081967213</v>
       </c>
       <c r="D82">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E82">
         <v>28</v>
       </c>
       <c r="F82">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G82">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H82">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,25 +2538,25 @@
         <v>0.082</v>
       </c>
       <c r="B83">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C83">
         <v>0.4262295081967213</v>
       </c>
       <c r="D83">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E83">
         <v>28</v>
       </c>
       <c r="F83">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G83">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H83">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,25 +2564,25 @@
         <v>0.083</v>
       </c>
       <c r="B84">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C84">
         <v>0.4262295081967213</v>
       </c>
       <c r="D84">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E84">
         <v>28</v>
       </c>
       <c r="F84">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G84">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H84">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,25 +2590,25 @@
         <v>0.08400000000000001</v>
       </c>
       <c r="B85">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C85">
         <v>0.4262295081967213</v>
       </c>
       <c r="D85">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E85">
         <v>28</v>
       </c>
       <c r="F85">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G85">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H85">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,25 +2616,25 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="B86">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C86">
         <v>0.4262295081967213</v>
       </c>
       <c r="D86">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E86">
         <v>28</v>
       </c>
       <c r="F86">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G86">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H86">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,25 +2642,25 @@
         <v>0.08600000000000001</v>
       </c>
       <c r="B87">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C87">
         <v>0.4262295081967213</v>
       </c>
       <c r="D87">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E87">
         <v>28</v>
       </c>
       <c r="F87">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G87">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H87">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,25 +2668,25 @@
         <v>0.08700000000000001</v>
       </c>
       <c r="B88">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C88">
         <v>0.4262295081967213</v>
       </c>
       <c r="D88">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E88">
         <v>28</v>
       </c>
       <c r="F88">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G88">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H88">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,25 +2694,25 @@
         <v>0.08799999999999999</v>
       </c>
       <c r="B89">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C89">
         <v>0.4262295081967213</v>
       </c>
       <c r="D89">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E89">
         <v>28</v>
       </c>
       <c r="F89">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G89">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H89">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,25 +2720,25 @@
         <v>0.089</v>
       </c>
       <c r="B90">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C90">
         <v>0.4262295081967213</v>
       </c>
       <c r="D90">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E90">
         <v>28</v>
       </c>
       <c r="F90">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G90">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H90">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,25 +2746,25 @@
         <v>0.09</v>
       </c>
       <c r="B91">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C91">
         <v>0.4262295081967213</v>
       </c>
       <c r="D91">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E91">
         <v>28</v>
       </c>
       <c r="F91">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G91">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H91">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,25 +2772,25 @@
         <v>0.091</v>
       </c>
       <c r="B92">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C92">
         <v>0.4262295081967213</v>
       </c>
       <c r="D92">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E92">
         <v>28</v>
       </c>
       <c r="F92">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G92">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H92">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,25 +2798,25 @@
         <v>0.092</v>
       </c>
       <c r="B93">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C93">
         <v>0.4262295081967213</v>
       </c>
       <c r="D93">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E93">
         <v>28</v>
       </c>
       <c r="F93">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G93">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H93">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2824,25 +2824,25 @@
         <v>0.093</v>
       </c>
       <c r="B94">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C94">
         <v>0.4262295081967213</v>
       </c>
       <c r="D94">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E94">
         <v>28</v>
       </c>
       <c r="F94">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G94">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H94">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2850,25 +2850,25 @@
         <v>0.094</v>
       </c>
       <c r="B95">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C95">
         <v>0.4262295081967213</v>
       </c>
       <c r="D95">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E95">
         <v>28</v>
       </c>
       <c r="F95">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G95">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H95">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2876,25 +2876,25 @@
         <v>0.095</v>
       </c>
       <c r="B96">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C96">
         <v>0.4262295081967213</v>
       </c>
       <c r="D96">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E96">
         <v>28</v>
       </c>
       <c r="F96">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G96">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H96">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2902,25 +2902,25 @@
         <v>0.096</v>
       </c>
       <c r="B97">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C97">
         <v>0.4262295081967213</v>
       </c>
       <c r="D97">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E97">
         <v>28</v>
       </c>
       <c r="F97">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G97">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H97">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2928,25 +2928,25 @@
         <v>0.097</v>
       </c>
       <c r="B98">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C98">
         <v>0.4262295081967213</v>
       </c>
       <c r="D98">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E98">
         <v>28</v>
       </c>
       <c r="F98">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G98">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H98">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2954,25 +2954,25 @@
         <v>0.098</v>
       </c>
       <c r="B99">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C99">
         <v>0.4262295081967213</v>
       </c>
       <c r="D99">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E99">
         <v>28</v>
       </c>
       <c r="F99">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G99">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H99">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2980,25 +2980,25 @@
         <v>0.099</v>
       </c>
       <c r="B100">
-        <v>0.2385321100917431</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="C100">
         <v>0.4262295081967213</v>
       </c>
       <c r="D100">
-        <v>0.3058823529411765</v>
+        <v>0.3537414965986394</v>
       </c>
       <c r="E100">
         <v>28</v>
       </c>
       <c r="F100">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G100">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H100">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added graph results for threshold
</commit_message>
<xml_diff>
--- a/analysis/edcr/Results.xlsx
+++ b/analysis/edcr/Results.xlsx
@@ -432,13 +432,13 @@
         <v>0.001</v>
       </c>
       <c r="B2">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C2">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D2">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -458,13 +458,13 @@
         <v>0.002</v>
       </c>
       <c r="B3">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C3">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D3">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -484,13 +484,13 @@
         <v>0.003</v>
       </c>
       <c r="B4">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C4">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D4">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -510,13 +510,13 @@
         <v>0.004</v>
       </c>
       <c r="B5">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C5">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D5">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -536,13 +536,13 @@
         <v>0.005</v>
       </c>
       <c r="B6">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C6">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D6">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -562,13 +562,13 @@
         <v>0.006</v>
       </c>
       <c r="B7">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C7">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D7">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -588,13 +588,13 @@
         <v>0.007</v>
       </c>
       <c r="B8">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C8">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D8">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -614,13 +614,13 @@
         <v>0.008</v>
       </c>
       <c r="B9">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C9">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D9">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -640,13 +640,13 @@
         <v>0.009000000000000001</v>
       </c>
       <c r="B10">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C10">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D10">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -666,13 +666,13 @@
         <v>0.01</v>
       </c>
       <c r="B11">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C11">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D11">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -692,13 +692,13 @@
         <v>0.011</v>
       </c>
       <c r="B12">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C12">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D12">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -718,13 +718,13 @@
         <v>0.012</v>
       </c>
       <c r="B13">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C13">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D13">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -744,13 +744,13 @@
         <v>0.013</v>
       </c>
       <c r="B14">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C14">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D14">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -770,13 +770,13 @@
         <v>0.014</v>
       </c>
       <c r="B15">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C15">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D15">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -796,13 +796,13 @@
         <v>0.015</v>
       </c>
       <c r="B16">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C16">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D16">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -822,13 +822,13 @@
         <v>0.016</v>
       </c>
       <c r="B17">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C17">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D17">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -848,13 +848,13 @@
         <v>0.017</v>
       </c>
       <c r="B18">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C18">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D18">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -874,13 +874,13 @@
         <v>0.018</v>
       </c>
       <c r="B19">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C19">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D19">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -900,13 +900,13 @@
         <v>0.019</v>
       </c>
       <c r="B20">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C20">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D20">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -926,13 +926,13 @@
         <v>0.02</v>
       </c>
       <c r="B21">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C21">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D21">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -952,13 +952,13 @@
         <v>0.021</v>
       </c>
       <c r="B22">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C22">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D22">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -978,13 +978,13 @@
         <v>0.022</v>
       </c>
       <c r="B23">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C23">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D23">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1004,13 +1004,13 @@
         <v>0.023</v>
       </c>
       <c r="B24">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C24">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D24">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1030,13 +1030,13 @@
         <v>0.024</v>
       </c>
       <c r="B25">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C25">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D25">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1056,13 +1056,13 @@
         <v>0.025</v>
       </c>
       <c r="B26">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C26">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D26">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1082,13 +1082,13 @@
         <v>0.026</v>
       </c>
       <c r="B27">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C27">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D27">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1108,13 +1108,13 @@
         <v>0.027</v>
       </c>
       <c r="B28">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C28">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D28">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1134,13 +1134,13 @@
         <v>0.028</v>
       </c>
       <c r="B29">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C29">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D29">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1160,13 +1160,13 @@
         <v>0.029</v>
       </c>
       <c r="B30">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C30">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D30">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1186,13 +1186,13 @@
         <v>0.03</v>
       </c>
       <c r="B31">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C31">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D31">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1212,13 +1212,13 @@
         <v>0.031</v>
       </c>
       <c r="B32">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C32">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D32">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1238,13 +1238,13 @@
         <v>0.032</v>
       </c>
       <c r="B33">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C33">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D33">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1264,13 +1264,13 @@
         <v>0.033</v>
       </c>
       <c r="B34">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C34">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D34">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1290,13 +1290,13 @@
         <v>0.034</v>
       </c>
       <c r="B35">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C35">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D35">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1316,13 +1316,13 @@
         <v>0.035</v>
       </c>
       <c r="B36">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C36">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D36">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1342,13 +1342,13 @@
         <v>0.036</v>
       </c>
       <c r="B37">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C37">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D37">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1368,13 +1368,13 @@
         <v>0.037</v>
       </c>
       <c r="B38">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C38">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D38">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1394,13 +1394,13 @@
         <v>0.038</v>
       </c>
       <c r="B39">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C39">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D39">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1420,13 +1420,13 @@
         <v>0.039</v>
       </c>
       <c r="B40">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C40">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D40">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1446,13 +1446,13 @@
         <v>0.04</v>
       </c>
       <c r="B41">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C41">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D41">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1472,13 +1472,13 @@
         <v>0.041</v>
       </c>
       <c r="B42">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C42">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D42">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1498,13 +1498,13 @@
         <v>0.042</v>
       </c>
       <c r="B43">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C43">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D43">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1524,13 +1524,13 @@
         <v>0.043</v>
       </c>
       <c r="B44">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C44">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D44">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1550,13 +1550,13 @@
         <v>0.044</v>
       </c>
       <c r="B45">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C45">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D45">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1576,13 +1576,13 @@
         <v>0.045</v>
       </c>
       <c r="B46">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C46">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D46">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1602,13 +1602,13 @@
         <v>0.046</v>
       </c>
       <c r="B47">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C47">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D47">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1628,13 +1628,13 @@
         <v>0.047</v>
       </c>
       <c r="B48">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C48">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D48">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -1654,13 +1654,13 @@
         <v>0.048</v>
       </c>
       <c r="B49">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C49">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D49">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1680,13 +1680,13 @@
         <v>0.049</v>
       </c>
       <c r="B50">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C50">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D50">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -1706,13 +1706,13 @@
         <v>0.05</v>
       </c>
       <c r="B51">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C51">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D51">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -1732,13 +1732,13 @@
         <v>0.051</v>
       </c>
       <c r="B52">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C52">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D52">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -1758,13 +1758,13 @@
         <v>0.052</v>
       </c>
       <c r="B53">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C53">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D53">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1784,13 +1784,13 @@
         <v>0.053</v>
       </c>
       <c r="B54">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C54">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D54">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -1810,13 +1810,13 @@
         <v>0.054</v>
       </c>
       <c r="B55">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C55">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D55">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1836,13 +1836,13 @@
         <v>0.055</v>
       </c>
       <c r="B56">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C56">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D56">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -1862,13 +1862,13 @@
         <v>0.056</v>
       </c>
       <c r="B57">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C57">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D57">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -1888,13 +1888,13 @@
         <v>0.057</v>
       </c>
       <c r="B58">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C58">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D58">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -1914,13 +1914,13 @@
         <v>0.058</v>
       </c>
       <c r="B59">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C59">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D59">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -1940,13 +1940,13 @@
         <v>0.059</v>
       </c>
       <c r="B60">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C60">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D60">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -1966,13 +1966,13 @@
         <v>0.06</v>
       </c>
       <c r="B61">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C61">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D61">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -1992,13 +1992,13 @@
         <v>0.061</v>
       </c>
       <c r="B62">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C62">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D62">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -2018,13 +2018,13 @@
         <v>0.062</v>
       </c>
       <c r="B63">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C63">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D63">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -2044,13 +2044,13 @@
         <v>0.063</v>
       </c>
       <c r="B64">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C64">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D64">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -2070,13 +2070,13 @@
         <v>0.064</v>
       </c>
       <c r="B65">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C65">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D65">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2096,13 +2096,13 @@
         <v>0.065</v>
       </c>
       <c r="B66">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C66">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D66">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -2122,13 +2122,13 @@
         <v>0.066</v>
       </c>
       <c r="B67">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C67">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D67">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -2148,13 +2148,13 @@
         <v>0.067</v>
       </c>
       <c r="B68">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C68">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D68">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -2174,13 +2174,13 @@
         <v>0.068</v>
       </c>
       <c r="B69">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C69">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D69">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -2200,13 +2200,13 @@
         <v>0.06900000000000001</v>
       </c>
       <c r="B70">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C70">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D70">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -2226,13 +2226,13 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="B71">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C71">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D71">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -2252,13 +2252,13 @@
         <v>0.07100000000000001</v>
       </c>
       <c r="B72">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C72">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D72">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -2278,13 +2278,13 @@
         <v>0.07200000000000001</v>
       </c>
       <c r="B73">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C73">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D73">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -2304,13 +2304,13 @@
         <v>0.073</v>
       </c>
       <c r="B74">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C74">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D74">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -2330,13 +2330,13 @@
         <v>0.074</v>
       </c>
       <c r="B75">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C75">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D75">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -2356,13 +2356,13 @@
         <v>0.075</v>
       </c>
       <c r="B76">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C76">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D76">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -2382,13 +2382,13 @@
         <v>0.076</v>
       </c>
       <c r="B77">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C77">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D77">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -2408,13 +2408,13 @@
         <v>0.077</v>
       </c>
       <c r="B78">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C78">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D78">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -2434,13 +2434,13 @@
         <v>0.078</v>
       </c>
       <c r="B79">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C79">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D79">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -2460,13 +2460,13 @@
         <v>0.079</v>
       </c>
       <c r="B80">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C80">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D80">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -2486,13 +2486,13 @@
         <v>0.08</v>
       </c>
       <c r="B81">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C81">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D81">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -2512,13 +2512,13 @@
         <v>0.081</v>
       </c>
       <c r="B82">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C82">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D82">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2538,13 +2538,13 @@
         <v>0.082</v>
       </c>
       <c r="B83">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C83">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D83">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -2564,13 +2564,13 @@
         <v>0.083</v>
       </c>
       <c r="B84">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C84">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D84">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -2590,13 +2590,13 @@
         <v>0.08400000000000001</v>
       </c>
       <c r="B85">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C85">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D85">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -2616,13 +2616,13 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="B86">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C86">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D86">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -2642,13 +2642,13 @@
         <v>0.08600000000000001</v>
       </c>
       <c r="B87">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C87">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D87">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -2668,13 +2668,13 @@
         <v>0.08700000000000001</v>
       </c>
       <c r="B88">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C88">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D88">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -2694,13 +2694,13 @@
         <v>0.08799999999999999</v>
       </c>
       <c r="B89">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C89">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D89">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E89">
         <v>0</v>
@@ -2720,13 +2720,13 @@
         <v>0.089</v>
       </c>
       <c r="B90">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C90">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D90">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -2746,13 +2746,13 @@
         <v>0.09</v>
       </c>
       <c r="B91">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C91">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D91">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -2772,13 +2772,13 @@
         <v>0.091</v>
       </c>
       <c r="B92">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C92">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D92">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -2798,13 +2798,13 @@
         <v>0.092</v>
       </c>
       <c r="B93">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C93">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D93">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -2824,13 +2824,13 @@
         <v>0.093</v>
       </c>
       <c r="B94">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C94">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D94">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -2850,13 +2850,13 @@
         <v>0.094</v>
       </c>
       <c r="B95">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C95">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D95">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -2876,13 +2876,13 @@
         <v>0.095</v>
       </c>
       <c r="B96">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C96">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D96">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -2902,13 +2902,13 @@
         <v>0.096</v>
       </c>
       <c r="B97">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C97">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D97">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -2928,13 +2928,13 @@
         <v>0.097</v>
       </c>
       <c r="B98">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C98">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D98">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E98">
         <v>0</v>
@@ -2954,13 +2954,13 @@
         <v>0.098</v>
       </c>
       <c r="B99">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C99">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D99">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E99">
         <v>0</v>
@@ -2980,13 +2980,13 @@
         <v>0.099</v>
       </c>
       <c r="B100">
-        <v>0.1146245059288538</v>
+        <v>0.625</v>
       </c>
       <c r="C100">
-        <v>0.6444444444444445</v>
+        <v>0.08196721311475409</v>
       </c>
       <c r="D100">
-        <v>0.1946308724832215</v>
+        <v>0.144927536231884</v>
       </c>
       <c r="E100">
         <v>0</v>

</xml_diff>

<commit_message>
feat: added new copper results
</commit_message>
<xml_diff>
--- a/analysis/edcr/Results.xlsx
+++ b/analysis/edcr/Results.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -476,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -502,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -554,7 +554,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -580,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -606,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -736,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -840,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -863,10 +863,10 @@
         <v>94</v>
       </c>
       <c r="G18">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H18">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -889,10 +889,10 @@
         <v>94</v>
       </c>
       <c r="G19">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H19">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -915,10 +915,10 @@
         <v>94</v>
       </c>
       <c r="G20">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H20">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -941,10 +941,10 @@
         <v>94</v>
       </c>
       <c r="G21">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H21">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -967,10 +967,10 @@
         <v>94</v>
       </c>
       <c r="G22">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H22">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -993,10 +993,10 @@
         <v>94</v>
       </c>
       <c r="G23">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H23">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1019,10 +1019,10 @@
         <v>94</v>
       </c>
       <c r="G24">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H24">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1045,10 +1045,10 @@
         <v>94</v>
       </c>
       <c r="G25">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H25">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1071,10 +1071,10 @@
         <v>94</v>
       </c>
       <c r="G26">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H26">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1097,10 +1097,10 @@
         <v>94</v>
       </c>
       <c r="G27">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H27">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1123,10 +1123,10 @@
         <v>94</v>
       </c>
       <c r="G28">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H28">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1149,10 +1149,10 @@
         <v>94</v>
       </c>
       <c r="G29">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H29">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1175,10 +1175,10 @@
         <v>94</v>
       </c>
       <c r="G30">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H30">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1201,10 +1201,10 @@
         <v>94</v>
       </c>
       <c r="G31">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H31">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1227,10 +1227,10 @@
         <v>94</v>
       </c>
       <c r="G32">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H32">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1253,10 +1253,10 @@
         <v>94</v>
       </c>
       <c r="G33">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H33">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1279,10 +1279,10 @@
         <v>94</v>
       </c>
       <c r="G34">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H34">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1305,10 +1305,10 @@
         <v>94</v>
       </c>
       <c r="G35">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H35">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1331,10 +1331,10 @@
         <v>94</v>
       </c>
       <c r="G36">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H36">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1357,10 +1357,10 @@
         <v>94</v>
       </c>
       <c r="G37">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H37">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1383,10 +1383,10 @@
         <v>94</v>
       </c>
       <c r="G38">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H38">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1409,10 +1409,10 @@
         <v>94</v>
       </c>
       <c r="G39">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H39">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1435,10 +1435,10 @@
         <v>94</v>
       </c>
       <c r="G40">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H40">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1461,10 +1461,10 @@
         <v>94</v>
       </c>
       <c r="G41">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H41">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1487,10 +1487,10 @@
         <v>94</v>
       </c>
       <c r="G42">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H42">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1513,10 +1513,10 @@
         <v>94</v>
       </c>
       <c r="G43">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H43">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1539,10 +1539,10 @@
         <v>94</v>
       </c>
       <c r="G44">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H44">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1565,10 +1565,10 @@
         <v>94</v>
       </c>
       <c r="G45">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H45">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1591,10 +1591,10 @@
         <v>94</v>
       </c>
       <c r="G46">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H46">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1617,10 +1617,10 @@
         <v>94</v>
       </c>
       <c r="G47">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H47">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1643,10 +1643,10 @@
         <v>94</v>
       </c>
       <c r="G48">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H48">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1669,10 +1669,10 @@
         <v>94</v>
       </c>
       <c r="G49">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H49">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1695,10 +1695,10 @@
         <v>94</v>
       </c>
       <c r="G50">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H50">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1721,10 +1721,10 @@
         <v>94</v>
       </c>
       <c r="G51">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H51">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1747,10 +1747,10 @@
         <v>94</v>
       </c>
       <c r="G52">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H52">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1773,10 +1773,10 @@
         <v>94</v>
       </c>
       <c r="G53">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H53">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1799,10 +1799,10 @@
         <v>94</v>
       </c>
       <c r="G54">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H54">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1825,10 +1825,10 @@
         <v>94</v>
       </c>
       <c r="G55">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H55">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1851,10 +1851,10 @@
         <v>94</v>
       </c>
       <c r="G56">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H56">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1877,10 +1877,10 @@
         <v>94</v>
       </c>
       <c r="G57">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H57">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1903,10 +1903,10 @@
         <v>94</v>
       </c>
       <c r="G58">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H58">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1929,10 +1929,10 @@
         <v>94</v>
       </c>
       <c r="G59">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H59">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1955,10 +1955,10 @@
         <v>94</v>
       </c>
       <c r="G60">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H60">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1981,10 +1981,10 @@
         <v>94</v>
       </c>
       <c r="G61">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H61">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2007,10 +2007,10 @@
         <v>94</v>
       </c>
       <c r="G62">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H62">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2033,10 +2033,10 @@
         <v>94</v>
       </c>
       <c r="G63">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H63">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2059,10 +2059,10 @@
         <v>94</v>
       </c>
       <c r="G64">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H64">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2085,10 +2085,10 @@
         <v>94</v>
       </c>
       <c r="G65">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H65">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2111,10 +2111,10 @@
         <v>94</v>
       </c>
       <c r="G66">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H66">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2137,10 +2137,10 @@
         <v>94</v>
       </c>
       <c r="G67">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H67">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2163,10 +2163,10 @@
         <v>94</v>
       </c>
       <c r="G68">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H68">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2189,10 +2189,10 @@
         <v>94</v>
       </c>
       <c r="G69">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H69">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2215,10 +2215,10 @@
         <v>94</v>
       </c>
       <c r="G70">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H70">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2241,10 +2241,10 @@
         <v>94</v>
       </c>
       <c r="G71">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H71">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2267,10 +2267,10 @@
         <v>94</v>
       </c>
       <c r="G72">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H72">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2293,10 +2293,10 @@
         <v>94</v>
       </c>
       <c r="G73">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H73">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2319,10 +2319,10 @@
         <v>94</v>
       </c>
       <c r="G74">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H74">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2345,10 +2345,10 @@
         <v>94</v>
       </c>
       <c r="G75">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H75">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2371,10 +2371,10 @@
         <v>94</v>
       </c>
       <c r="G76">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H76">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2397,10 +2397,10 @@
         <v>94</v>
       </c>
       <c r="G77">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H77">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2423,10 +2423,10 @@
         <v>94</v>
       </c>
       <c r="G78">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H78">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2449,10 +2449,10 @@
         <v>94</v>
       </c>
       <c r="G79">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H79">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2475,10 +2475,10 @@
         <v>94</v>
       </c>
       <c r="G80">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H80">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2501,10 +2501,10 @@
         <v>94</v>
       </c>
       <c r="G81">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H81">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2527,10 +2527,10 @@
         <v>94</v>
       </c>
       <c r="G82">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H82">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2553,10 +2553,10 @@
         <v>94</v>
       </c>
       <c r="G83">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H83">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2579,10 +2579,10 @@
         <v>94</v>
       </c>
       <c r="G84">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H84">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2605,10 +2605,10 @@
         <v>94</v>
       </c>
       <c r="G85">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H85">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2631,10 +2631,10 @@
         <v>94</v>
       </c>
       <c r="G86">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H86">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2657,10 +2657,10 @@
         <v>94</v>
       </c>
       <c r="G87">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H87">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2683,10 +2683,10 @@
         <v>94</v>
       </c>
       <c r="G88">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H88">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2709,10 +2709,10 @@
         <v>94</v>
       </c>
       <c r="G89">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H89">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2735,10 +2735,10 @@
         <v>94</v>
       </c>
       <c r="G90">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H90">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2761,10 +2761,10 @@
         <v>94</v>
       </c>
       <c r="G91">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H91">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2787,10 +2787,10 @@
         <v>94</v>
       </c>
       <c r="G92">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H92">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2813,10 +2813,10 @@
         <v>94</v>
       </c>
       <c r="G93">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H93">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2839,10 +2839,10 @@
         <v>94</v>
       </c>
       <c r="G94">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H94">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2865,10 +2865,10 @@
         <v>94</v>
       </c>
       <c r="G95">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H95">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2891,10 +2891,10 @@
         <v>94</v>
       </c>
       <c r="G96">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H96">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2917,10 +2917,10 @@
         <v>94</v>
       </c>
       <c r="G97">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H97">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2943,10 +2943,10 @@
         <v>94</v>
       </c>
       <c r="G98">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H98">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2969,10 +2969,10 @@
         <v>94</v>
       </c>
       <c r="G99">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H99">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2995,10 +2995,10 @@
         <v>94</v>
       </c>
       <c r="G100">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H100">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>